<commit_message>
- Teilelisten aktualisiert - Exceldokument "Bestellisten.xlsx" in Verzeichnis doc aufgesetzt
</commit_message>
<xml_diff>
--- a/kicad_drvbatswitch/drvbatswitch_Teileliste.xlsx
+++ b/kicad_drvbatswitch/drvbatswitch_Teileliste.xlsx
@@ -1,25 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17030"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Andreas\Documents\Uni\Job_IAT\KiCad\Schalter_Fahrakku\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Andreas\Documents\Uni\Job_IAT\basicboard\kicad_drvbatswitch\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="7935"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9555" windowHeight="2940"/>
   </bookViews>
   <sheets>
-    <sheet name="Schalter_Fahrakku" sheetId="1" r:id="rId1"/>
+    <sheet name="drvbatswitch" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">drvbatswitch!$A$1:$K$1</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="77">
   <si>
     <t>Reference</t>
   </si>
@@ -27,6 +30,9 @@
     <t xml:space="preserve"> Value</t>
   </si>
   <si>
+    <t xml:space="preserve"> Footprint</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Datasheet</t>
   </si>
   <si>
@@ -54,6 +60,9 @@
     <t>IRLML6344</t>
   </si>
   <si>
+    <t>TO_SOT_Packages_SMD:SOT-23</t>
+  </si>
+  <si>
     <t>http://www.farnell.com/datasheets/1911844.pdf</t>
   </si>
   <si>
@@ -72,6 +81,9 @@
     <t>IPD90P03</t>
   </si>
   <si>
+    <t>TO_SOT_Packages_SMD:TO-252-2Lead</t>
+  </si>
+  <si>
     <t>http://www.farnell.com/datasheets/1932578.pdf</t>
   </si>
   <si>
@@ -81,13 +93,28 @@
     <t>TO252</t>
   </si>
   <si>
-    <t>uC_IN1</t>
-  </si>
-  <si>
-    <t>SIL 3</t>
-  </si>
-  <si>
-    <t>1x3 Header</t>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>uC_IN</t>
+  </si>
+  <si>
+    <t>Custom:PS25_3W</t>
+  </si>
+  <si>
+    <t>http://cdn-reichelt.de/documents/datenblatt/C151/PS25_xxWBR.pdf</t>
+  </si>
+  <si>
+    <t>Reichelt</t>
+  </si>
+  <si>
+    <t>PS 25/3W BR</t>
+  </si>
+  <si>
+    <t>http://www.reichelt.de/PS-25-3W-BR/3/index.html?ACTION=3&amp;LA=446&amp;ARTICLE=14828&amp;artnr=PS+25%2F3W+BR&amp;SEARCH=PS+25</t>
+  </si>
+  <si>
+    <t>1x3 Angled</t>
   </si>
   <si>
     <t>C1</t>
@@ -96,6 +123,9 @@
     <t>100n</t>
   </si>
   <si>
+    <t>Capacitors_SMD:C_0603_HandSoldering</t>
+  </si>
+  <si>
     <t>4V</t>
   </si>
   <si>
@@ -105,6 +135,9 @@
     <t>10k</t>
   </si>
   <si>
+    <t>Resistors_SMD:R_0603_HandSoldering</t>
+  </si>
+  <si>
     <t>R2</t>
   </si>
   <si>
@@ -115,6 +148,111 @@
   </si>
   <si>
     <t>10V</t>
+  </si>
+  <si>
+    <t>PD1</t>
+  </si>
+  <si>
+    <t>Hole</t>
+  </si>
+  <si>
+    <t>Custom:MountingHole_3.3mm_M3</t>
+  </si>
+  <si>
+    <t>PD2</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>3k6</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>V_IN+</t>
+  </si>
+  <si>
+    <t>Custom:Pad_SMD_3.5x10</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>V_IN-</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>V_OUT+</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>V_OUT-</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>Custom:LED_0603_HandSoldering</t>
+  </si>
+  <si>
+    <t>PD6</t>
+  </si>
+  <si>
+    <t>Custom:Hole_3mm</t>
+  </si>
+  <si>
+    <t>PD10</t>
+  </si>
+  <si>
+    <t>PD14</t>
+  </si>
+  <si>
+    <t>PD18</t>
+  </si>
+  <si>
+    <t>PD5</t>
+  </si>
+  <si>
+    <t>PD9</t>
+  </si>
+  <si>
+    <t>PD13</t>
+  </si>
+  <si>
+    <t>PD17</t>
+  </si>
+  <si>
+    <t>PD4</t>
+  </si>
+  <si>
+    <t>PD8</t>
+  </si>
+  <si>
+    <t>PD12</t>
+  </si>
+  <si>
+    <t>PD16</t>
+  </si>
+  <si>
+    <t>PD3</t>
+  </si>
+  <si>
+    <t>PD7</t>
+  </si>
+  <si>
+    <t>PD11</t>
+  </si>
+  <si>
+    <t>PD15</t>
   </si>
 </sst>
 </file>
@@ -955,15 +1093,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -971,132 +1109,438 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2">
+        <v>1857299</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3">
+        <v>2480839</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3">
+        <v>1.39</v>
+      </c>
+      <c r="J3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
         <v>23</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>24</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4">
+        <v>0.42</v>
+      </c>
+      <c r="J4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4">
-        <v>1857299</v>
-      </c>
-      <c r="G4">
-        <v>0.16800000000000001</v>
-      </c>
-      <c r="H4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
       <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5">
-        <v>2480839</v>
-      </c>
-      <c r="G5">
-        <v>1.39</v>
-      </c>
-      <c r="H5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+      <c r="J6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+      <c r="J7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="J10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="J11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="J13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="J14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
+      <c r="J15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" t="s">
+        <v>58</v>
+      </c>
+      <c r="J16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="J17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="J18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="J19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="J20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="J21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="J22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+      <c r="J23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+      <c r="J24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" t="s">
+        <v>43</v>
+      </c>
+      <c r="J25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" t="s">
+        <v>43</v>
+      </c>
+      <c r="J26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" t="s">
+        <v>43</v>
+      </c>
+      <c r="J27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" t="s">
+        <v>43</v>
+      </c>
+      <c r="J28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" t="s">
+        <v>43</v>
+      </c>
+      <c r="J29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" t="s">
+        <v>43</v>
+      </c>
+      <c r="J30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" t="s">
+        <v>43</v>
+      </c>
+      <c r="J31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" t="s">
+        <v>43</v>
+      </c>
+      <c r="J32" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:I16">
-    <sortCondition ref="A1"/>
-  </sortState>
+  <autoFilter ref="A1:K1">
+    <sortState ref="A2:J32">
+      <sortCondition ref="F1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>